<commit_message>
agregar poliza editable. filtrar en busqueda
</commit_message>
<xml_diff>
--- a/templates/plantilla-cartera.xlsx
+++ b/templates/plantilla-cartera.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilio\Documents\NetBeansProjects\ControlCartera\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emilio\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B58A067-6633-4CB1-9ABA-55ACA1034E50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F99199-1B6D-473E-8325-68F9E6E87E09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="META" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="META" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -265,6 +265,36 @@
   </si>
   <si>
     <t>Moral</t>
+  </si>
+  <si>
+    <t>GMM</t>
+  </si>
+  <si>
+    <t>DEDUCIBLE</t>
+  </si>
+  <si>
+    <t>SUMA ASEGURADA</t>
+  </si>
+  <si>
+    <t>COASEGURO</t>
+  </si>
+  <si>
+    <t>VIDA</t>
+  </si>
+  <si>
+    <t>SUMA ASEGURADA AUTOS</t>
+  </si>
+  <si>
+    <t>Factura</t>
+  </si>
+  <si>
+    <t>Comercial</t>
+  </si>
+  <si>
+    <t>CONTRATANTE</t>
+  </si>
+  <si>
+    <t>AUTOS/FLOTILLA</t>
   </si>
 </sst>
 </file>
@@ -275,7 +305,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -303,8 +333,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -317,8 +361,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -341,23 +403,222 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,14 +647,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{30F60C86-D5B0-4A7F-AF28-2BF3E639D37B}" name="Tabla4" displayName="Tabla4" ref="B1:F1048576" totalsRowShown="0">
-  <autoFilter ref="B1:F1048576" xr:uid="{E035FA9D-0EB0-4DE5-A313-D175098B16CE}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{30F60C86-D5B0-4A7F-AF28-2BF3E639D37B}" name="Tabla4" displayName="Tabla4" ref="B1:G1048576" totalsRowShown="0">
+  <autoFilter ref="B1:G1048576" xr:uid="{E035FA9D-0EB0-4DE5-A313-D175098B16CE}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{8AA8FD79-530F-47E7-8B21-2D955686CE53}" name="ASEGURADORA"/>
     <tableColumn id="2" xr3:uid="{A3853F89-7953-41CA-9D47-CDADA36C2592}" name="FORMA DE PAGO"/>
     <tableColumn id="3" xr3:uid="{FCE65D0F-545F-4008-82B0-3556176ACA4F}" name="CONDUCTO DE COBRO"/>
     <tableColumn id="4" xr3:uid="{D97BE710-C459-4617-ADDF-AF0D01F94A38}" name="MONEDA"/>
     <tableColumn id="5" xr3:uid="{A4EC0CBF-1F90-4353-B410-AD4612F1BD82}" name="TIPO DE PERSONA"/>
+    <tableColumn id="6" xr3:uid="{23C7FA4B-8C9B-41BC-9CEB-50D44EA02DBC}" name="SUMA ASEGURADA AUTOS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -696,90 +958,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="1026" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1"/>
+    <col min="18" max="18" width="17.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" style="6" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="1026" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="W1" s="20"/>
+    </row>
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D2" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>13</v>
+      <c r="R2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="S2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576" xr:uid="{41D0734E-7876-4AD2-A4CF-52B7C08D3595}">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="M3:M1048576" xr:uid="{41D0734E-7876-4AD2-A4CF-52B7C08D3595}">
       <formula1>0</formula1>
       <formula2>12</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{C6F737B1-0761-430B-9215-582FB8C1BF90}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576" xr:uid="{C6F737B1-0761-430B-9215-582FB8C1BF90}">
       <formula1>1</formula1>
       <formula2>73051</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1:O1048576" xr:uid="{BF16F016-118C-4E11-9EA7-A3AF74099C6E}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O1048576" xr:uid="{BF16F016-118C-4E11-9EA7-A3AF74099C6E}">
       <formula1>ISBLANK(O:O)=FALSE</formula1>
     </dataValidation>
   </dataValidations>
@@ -787,42 +1129,48 @@
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{825651D1-6CDA-4213-B584-D43FD1BB6986}">
           <x14:formula1>
             <xm:f>META!$B$2:$B$41</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>F3:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3C1973E2-BD4A-4C8D-84EE-6C75360160C1}">
           <x14:formula1>
             <xm:f>META!$A$2:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
+          <xm:sqref>G3:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{152E669C-46FC-437A-98C3-DFDE0D58DDDF}">
           <x14:formula1>
             <xm:f>META!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
+          <xm:sqref>I3:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3C2B387E-8C02-4567-88D1-C00539F0FCD0}">
           <x14:formula1>
             <xm:f>META!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J1:J1048576</xm:sqref>
+          <xm:sqref>J3:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BFB8895F-2A87-48E6-806E-5F2787B722C5}">
           <x14:formula1>
             <xm:f>META!$E$2:$E$5</xm:f>
           </x14:formula1>
-          <xm:sqref>L1:L1048576</xm:sqref>
+          <xm:sqref>W3:W1048576 S3:S1048576 L3:L1048576 Q3:Q1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C95BFF90-7BD2-41EE-A0B5-3139C1410D5E}">
           <x14:formula1>
             <xm:f>META!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>D3:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2D106F02-1CBC-49DE-B3DC-314EBC14AA58}">
+          <x14:formula1>
+            <xm:f>META!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>U3:U1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -832,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2C24031-08AB-42A7-BC1E-9CE9BD565327}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,9 +1192,10 @@
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -865,8 +1214,11 @@
       <c r="F1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -885,8 +1237,11 @@
       <c r="F2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -905,8 +1260,11 @@
       <c r="F3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -923,7 +1281,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -937,7 +1295,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -945,7 +1303,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -953,7 +1311,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>63</v>
       </c>
@@ -961,7 +1319,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -969,7 +1327,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -977,7 +1335,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>66</v>
       </c>
@@ -985,28 +1343,28 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>28</v>
       </c>

</xml_diff>